<commit_message>
chore: added boardup line in excel db
</commit_message>
<xml_diff>
--- a/public/assets/docs/glass_prices.xlsx
+++ b/public/assets/docs/glass_prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
   <si>
     <t xml:space="preserve">GLASS</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board Up</t>
   </si>
   <si>
     <t xml:space="preserve">1/8 CLEAR ANN</t>
@@ -893,67 +896,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1208,21 +1211,21 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A205" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C228" activeCellId="0" sqref="C228"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.62890625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="1" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1240,15 +1243,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="n">
-        <f aca="false">E2*2.3</f>
-        <v>6.325</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>2.75</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1256,13 +1254,13 @@
       </c>
       <c r="B3" s="5" t="n">
         <f aca="false">E3*2.3</f>
-        <v>14.168</v>
+        <v>6.325</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>6.16</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,13 +1299,13 @@
       </c>
       <c r="B6" s="5" t="n">
         <f aca="false">E6*2.3</f>
-        <v>37.72</v>
+        <v>14.168</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>16.4</v>
+        <v>6.16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,13 +1314,13 @@
       </c>
       <c r="B7" s="5" t="n">
         <f aca="false">E7*2.3</f>
-        <v>11.5</v>
+        <v>37.72</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>5</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1331,13 +1329,13 @@
       </c>
       <c r="B8" s="5" t="n">
         <f aca="false">E8*2.3</f>
-        <v>14.375</v>
+        <v>11.5</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>6.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,13 +1344,13 @@
       </c>
       <c r="B9" s="5" t="n">
         <f aca="false">E9*2.3</f>
-        <v>41.4</v>
+        <v>14.375</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>18</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,13 +1359,13 @@
       </c>
       <c r="B10" s="5" t="n">
         <f aca="false">E10*2.3</f>
-        <v>19.021</v>
+        <v>41.4</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>8.27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,13 +1374,13 @@
       </c>
       <c r="B11" s="5" t="n">
         <f aca="false">E11*2.3</f>
-        <v>14.352</v>
+        <v>19.021</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>6.24</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,13 +1389,13 @@
       </c>
       <c r="B12" s="5" t="n">
         <f aca="false">E12*2.3</f>
-        <v>17.595</v>
+        <v>14.352</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>7.65</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,13 +1404,13 @@
       </c>
       <c r="B13" s="5" t="n">
         <f aca="false">E13*2.3</f>
-        <v>9.108</v>
+        <v>17.595</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>3.96</v>
+        <v>7.65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,13 +1419,13 @@
       </c>
       <c r="B14" s="5" t="n">
         <f aca="false">E14*2.3</f>
-        <v>16.698</v>
+        <v>9.108</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>7.26</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1466,13 +1464,13 @@
       </c>
       <c r="B17" s="5" t="n">
         <f aca="false">E17*2.3</f>
-        <v>42.274</v>
+        <v>16.698</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>18.38</v>
+        <v>7.26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,13 +1479,13 @@
       </c>
       <c r="B18" s="5" t="n">
         <f aca="false">E18*2.3</f>
-        <v>14.95</v>
+        <v>42.274</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>6.5</v>
+        <v>18.38</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,13 +1494,13 @@
       </c>
       <c r="B19" s="5" t="n">
         <f aca="false">E19*2.3</f>
-        <v>18.975</v>
+        <v>14.95</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>8.25</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,28 +1509,28 @@
       </c>
       <c r="B20" s="5" t="n">
         <f aca="false">E20*2.3</f>
-        <v>22.195</v>
+        <v>18.975</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>9.65</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="5" t="n">
         <f aca="false">E21*2.3</f>
-        <v>16.284</v>
+        <v>22.195</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>7.08</v>
+        <v>9.65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1541,13 +1539,13 @@
       </c>
       <c r="B22" s="5" t="n">
         <f aca="false">E22*2.3</f>
-        <v>9.982</v>
+        <v>16.284</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>4.34</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1556,13 +1554,13 @@
       </c>
       <c r="B23" s="5" t="n">
         <f aca="false">E23*2.3</f>
-        <v>33.005</v>
+        <v>9.982</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>14.35</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1571,43 +1569,43 @@
       </c>
       <c r="B24" s="5" t="n">
         <f aca="false">E24*2.3</f>
-        <v>51.129</v>
+        <v>33.005</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>22.23</v>
+        <v>14.35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="5" t="n">
         <f aca="false">E25*2.3</f>
-        <v>21.85</v>
+        <v>51.129</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>9.5</v>
+        <v>22.23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="5" t="n">
         <f aca="false">E26*2.3</f>
-        <v>20.47</v>
+        <v>21.85</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>8.9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1616,13 +1614,13 @@
       </c>
       <c r="B27" s="5" t="n">
         <f aca="false">E27*2.3</f>
-        <v>33.925</v>
+        <v>20.47</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>14.75</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1631,13 +1629,13 @@
       </c>
       <c r="B28" s="5" t="n">
         <f aca="false">E28*2.3</f>
-        <v>10.051</v>
+        <v>33.925</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>4.37</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1646,13 +1644,13 @@
       </c>
       <c r="B29" s="5" t="n">
         <f aca="false">E29*2.3</f>
-        <v>49.22</v>
+        <v>10.051</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>21.4</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1661,13 +1659,13 @@
       </c>
       <c r="B30" s="5" t="n">
         <f aca="false">E30*2.3</f>
-        <v>11.891</v>
+        <v>49.22</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>5.17</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1676,13 +1674,13 @@
       </c>
       <c r="B31" s="5" t="n">
         <f aca="false">E31*2.3</f>
-        <v>37.099</v>
+        <v>11.891</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E31" s="7" t="n">
-        <v>16.13</v>
+      <c r="E31" s="5" t="n">
+        <v>5.17</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1691,13 +1689,13 @@
       </c>
       <c r="B32" s="5" t="n">
         <f aca="false">E32*2.3</f>
-        <v>26.45</v>
+        <v>37.099</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="E32" s="5" t="n">
-        <v>11.5</v>
+      <c r="E32" s="7" t="n">
+        <v>16.13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1706,13 +1704,13 @@
       </c>
       <c r="B33" s="5" t="n">
         <f aca="false">E33*2.3</f>
-        <v>23.575</v>
+        <v>26.45</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>10.25</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1721,13 +1719,13 @@
       </c>
       <c r="B34" s="5" t="n">
         <f aca="false">E34*2.3</f>
-        <v>37.95</v>
+        <v>23.575</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>16.5</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1736,13 +1734,13 @@
       </c>
       <c r="B35" s="5" t="n">
         <f aca="false">E35*2.3</f>
-        <v>15.571</v>
+        <v>37.95</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>6.77</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1751,13 +1749,13 @@
       </c>
       <c r="B36" s="5" t="n">
         <f aca="false">E36*2.3</f>
-        <v>61.525</v>
+        <v>15.571</v>
       </c>
       <c r="C36" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>26.75</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1766,13 +1764,13 @@
       </c>
       <c r="B37" s="5" t="n">
         <f aca="false">E37*2.3</f>
-        <v>11.178</v>
+        <v>61.525</v>
       </c>
       <c r="C37" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>4.86</v>
+        <v>26.75</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1781,13 +1779,13 @@
       </c>
       <c r="B38" s="5" t="n">
         <f aca="false">E38*2.3</f>
-        <v>18.4</v>
+        <v>11.178</v>
       </c>
       <c r="C38" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>8</v>
+        <v>4.86</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1826,13 +1824,13 @@
       </c>
       <c r="B41" s="5" t="n">
         <f aca="false">E41*2.3</f>
-        <v>32.062</v>
+        <v>18.4</v>
       </c>
       <c r="C41" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>13.94</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1841,43 +1839,43 @@
       </c>
       <c r="B42" s="5" t="n">
         <f aca="false">E42*2.3</f>
-        <v>13.271</v>
+        <v>32.062</v>
       </c>
       <c r="C42" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>5.77</v>
+        <v>13.94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B43" s="5" t="n">
         <f aca="false">E43*2.3</f>
-        <v>14.053</v>
+        <v>13.271</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>6.11</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="5" t="n">
         <f aca="false">E44*2.3</f>
-        <v>19.665</v>
+        <v>14.053</v>
       </c>
       <c r="C44" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>8.55</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1886,13 +1884,13 @@
       </c>
       <c r="B45" s="5" t="n">
         <f aca="false">E45*2.3</f>
-        <v>12.742</v>
+        <v>19.665</v>
       </c>
       <c r="C45" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>5.54</v>
+        <v>8.55</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1901,13 +1899,13 @@
       </c>
       <c r="B46" s="5" t="n">
         <f aca="false">E46*2.3</f>
-        <v>21.137</v>
+        <v>12.742</v>
       </c>
       <c r="C46" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>9.19</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1946,13 +1944,13 @@
       </c>
       <c r="B49" s="5" t="n">
         <f aca="false">E49*2.3</f>
-        <v>34.5</v>
+        <v>21.137</v>
       </c>
       <c r="C49" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>15</v>
+        <v>9.19</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1961,13 +1959,13 @@
       </c>
       <c r="B50" s="5" t="n">
         <f aca="false">E50*2.3</f>
-        <v>18.699</v>
+        <v>34.5</v>
       </c>
       <c r="C50" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>8.13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1976,13 +1974,13 @@
       </c>
       <c r="B51" s="5" t="n">
         <f aca="false">E51*2.3</f>
-        <v>20.125</v>
+        <v>18.699</v>
       </c>
       <c r="C51" s="3" t="n">
         <v>2.5</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>8.75</v>
+        <v>8.13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1991,13 +1989,13 @@
       </c>
       <c r="B52" s="5" t="n">
         <f aca="false">E52*2.3</f>
-        <v>11.339</v>
+        <v>20.125</v>
       </c>
       <c r="C52" s="3" t="n">
-        <v>3.3</v>
+        <v>2.5</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>4.93</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2006,13 +2004,13 @@
       </c>
       <c r="B53" s="5" t="n">
         <f aca="false">E53*2.3</f>
-        <v>26.726</v>
+        <v>11.339</v>
       </c>
       <c r="C53" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>11.62</v>
+        <v>4.93</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2021,13 +2019,13 @@
       </c>
       <c r="B54" s="5" t="n">
         <f aca="false">E54*2.3</f>
-        <v>17.25</v>
+        <v>26.726</v>
       </c>
       <c r="C54" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>7.5</v>
+        <v>11.62</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2066,13 +2064,13 @@
       </c>
       <c r="B57" s="5" t="n">
         <f aca="false">E57*2.3</f>
-        <v>54.326</v>
+        <v>17.25</v>
       </c>
       <c r="C57" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>23.62</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2081,13 +2079,13 @@
       </c>
       <c r="B58" s="5" t="n">
         <f aca="false">E58*2.3</f>
-        <v>39.836</v>
+        <v>54.326</v>
       </c>
       <c r="C58" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>17.32</v>
+        <v>23.62</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2111,13 +2109,13 @@
       </c>
       <c r="B60" s="5" t="n">
         <f aca="false">E60*2.3</f>
-        <v>25.852</v>
+        <v>39.836</v>
       </c>
       <c r="C60" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>11.24</v>
+        <v>17.32</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2126,13 +2124,13 @@
       </c>
       <c r="B61" s="5" t="n">
         <f aca="false">E61*2.3</f>
-        <v>16.008</v>
+        <v>25.852</v>
       </c>
       <c r="C61" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>6.96</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2141,13 +2139,13 @@
       </c>
       <c r="B62" s="5" t="n">
         <f aca="false">E62*2.3</f>
-        <v>55.476</v>
+        <v>16.008</v>
       </c>
       <c r="C62" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>24.12</v>
+        <v>6.96</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2156,13 +2154,13 @@
       </c>
       <c r="B63" s="5" t="n">
         <f aca="false">E63*2.3</f>
-        <v>98.003</v>
+        <v>55.476</v>
       </c>
       <c r="C63" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>42.61</v>
+        <v>24.12</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2171,13 +2169,13 @@
       </c>
       <c r="B64" s="5" t="n">
         <f aca="false">E64*2.3</f>
-        <v>13.225</v>
+        <v>98.003</v>
       </c>
       <c r="C64" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>5.75</v>
+        <v>42.61</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2186,13 +2184,13 @@
       </c>
       <c r="B65" s="5" t="n">
         <f aca="false">E65*2.3</f>
-        <v>28.152</v>
+        <v>13.225</v>
       </c>
       <c r="C65" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>12.24</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2201,13 +2199,13 @@
       </c>
       <c r="B66" s="5" t="n">
         <f aca="false">E66*2.3</f>
-        <v>20.608</v>
+        <v>28.152</v>
       </c>
       <c r="C66" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>8.96</v>
+        <v>12.24</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2246,13 +2244,13 @@
       </c>
       <c r="B69" s="5" t="n">
         <f aca="false">E69*2.3</f>
-        <v>60.904</v>
+        <v>20.608</v>
       </c>
       <c r="C69" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>26.48</v>
+        <v>8.96</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2261,13 +2259,13 @@
       </c>
       <c r="B70" s="5" t="n">
         <f aca="false">E70*2.3</f>
-        <v>42.228</v>
+        <v>60.904</v>
       </c>
       <c r="C70" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>18.36</v>
+        <v>26.48</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2291,13 +2289,13 @@
       </c>
       <c r="B72" s="5" t="n">
         <f aca="false">E72*2.3</f>
-        <v>28.474</v>
+        <v>42.228</v>
       </c>
       <c r="C72" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E72" s="5" t="n">
-        <v>12.38</v>
+        <v>18.36</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2306,13 +2304,13 @@
       </c>
       <c r="B73" s="5" t="n">
         <f aca="false">E73*2.3</f>
-        <v>60.858</v>
+        <v>28.474</v>
       </c>
       <c r="C73" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E73" s="5" t="n">
-        <v>26.46</v>
+        <v>12.38</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2321,13 +2319,13 @@
       </c>
       <c r="B74" s="5" t="n">
         <f aca="false">E74*2.3</f>
-        <v>28.083</v>
+        <v>60.858</v>
       </c>
       <c r="C74" s="3" t="n">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="E74" s="5" t="n">
-        <v>12.21</v>
+        <v>26.46</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2336,13 +2334,13 @@
       </c>
       <c r="B75" s="5" t="n">
         <f aca="false">E75*2.3</f>
-        <v>40.48</v>
+        <v>28.083</v>
       </c>
       <c r="C75" s="3" t="n">
         <v>5</v>
       </c>
       <c r="E75" s="5" t="n">
-        <v>17.6</v>
+        <v>12.21</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2381,13 +2379,13 @@
       </c>
       <c r="B78" s="5" t="n">
         <f aca="false">E78*2.3</f>
-        <v>36.8</v>
+        <v>40.48</v>
       </c>
       <c r="C78" s="3" t="n">
         <v>5</v>
       </c>
       <c r="E78" s="5" t="n">
-        <v>16</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2396,13 +2394,13 @@
       </c>
       <c r="B79" s="5" t="n">
         <f aca="false">E79*2.3</f>
-        <v>15.709</v>
+        <v>36.8</v>
       </c>
       <c r="C79" s="3" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="E79" s="5" t="n">
-        <v>6.83</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2411,13 +2409,13 @@
       </c>
       <c r="B80" s="5" t="n">
         <f aca="false">E80*2.3</f>
-        <v>39.192</v>
+        <v>15.709</v>
       </c>
       <c r="C80" s="3" t="n">
         <v>5.5</v>
       </c>
       <c r="E80" s="5" t="n">
-        <v>17.04</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2426,13 +2424,13 @@
       </c>
       <c r="B81" s="5" t="n">
         <f aca="false">E81*2.3</f>
-        <v>101.085</v>
+        <v>39.192</v>
       </c>
       <c r="C81" s="3" t="n">
         <v>5.5</v>
       </c>
       <c r="E81" s="5" t="n">
-        <v>43.95</v>
+        <v>17.04</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2441,13 +2439,13 @@
       </c>
       <c r="B82" s="5" t="n">
         <f aca="false">E82*2.3</f>
-        <v>37.582</v>
+        <v>101.085</v>
       </c>
       <c r="C82" s="3" t="n">
         <v>5.5</v>
       </c>
       <c r="E82" s="5" t="n">
-        <v>16.34</v>
+        <v>43.95</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2456,13 +2454,13 @@
       </c>
       <c r="B83" s="5" t="n">
         <f aca="false">E83*2.3</f>
-        <v>18.791</v>
+        <v>37.582</v>
       </c>
       <c r="C83" s="3" t="n">
         <v>5.5</v>
       </c>
       <c r="E83" s="5" t="n">
-        <v>8.17</v>
+        <v>16.34</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2471,13 +2469,13 @@
       </c>
       <c r="B84" s="5" t="n">
         <f aca="false">E84*2.3</f>
-        <v>43.7</v>
+        <v>18.791</v>
       </c>
       <c r="C84" s="3" t="n">
         <v>5.5</v>
       </c>
       <c r="E84" s="5" t="n">
-        <v>19</v>
+        <v>8.17</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2486,13 +2484,13 @@
       </c>
       <c r="B85" s="5" t="n">
         <f aca="false">E85*2.3</f>
-        <v>103.5</v>
+        <v>43.7</v>
       </c>
       <c r="C85" s="3" t="n">
         <v>5.5</v>
       </c>
       <c r="E85" s="5" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2501,13 +2499,13 @@
       </c>
       <c r="B86" s="5" t="n">
         <f aca="false">E86*2.3</f>
-        <v>41.929</v>
+        <v>103.5</v>
       </c>
       <c r="C86" s="3" t="n">
         <v>5.5</v>
       </c>
       <c r="E86" s="5" t="n">
-        <v>18.23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2516,13 +2514,13 @@
       </c>
       <c r="B87" s="5" t="n">
         <f aca="false">E87*2.3</f>
-        <v>26.22</v>
+        <v>41.929</v>
       </c>
       <c r="C87" s="3" t="n">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="E87" s="5" t="n">
-        <v>11.4</v>
+        <v>18.23</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2531,13 +2529,13 @@
       </c>
       <c r="B88" s="5" t="n">
         <f aca="false">E88*2.3</f>
-        <v>54.096</v>
+        <v>26.22</v>
       </c>
       <c r="C88" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E88" s="5" t="n">
-        <v>23.52</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2546,13 +2544,13 @@
       </c>
       <c r="B89" s="5" t="n">
         <f aca="false">E89*2.3</f>
-        <v>43.516</v>
+        <v>54.096</v>
       </c>
       <c r="C89" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E89" s="5" t="n">
-        <v>18.92</v>
+        <v>23.52</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2561,13 +2559,13 @@
       </c>
       <c r="B90" s="5" t="n">
         <f aca="false">E90*2.3</f>
-        <v>29.348</v>
+        <v>43.516</v>
       </c>
       <c r="C90" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E90" s="5" t="n">
-        <v>12.76</v>
+        <v>18.92</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2576,13 +2574,13 @@
       </c>
       <c r="B91" s="5" t="n">
         <f aca="false">E91*2.3</f>
-        <v>58.121</v>
+        <v>29.348</v>
       </c>
       <c r="C91" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E91" s="5" t="n">
-        <v>25.27</v>
+        <v>12.76</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2591,43 +2589,43 @@
       </c>
       <c r="B92" s="5" t="n">
         <f aca="false">E92*2.3</f>
-        <v>47.518</v>
+        <v>58.121</v>
       </c>
       <c r="C92" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E92" s="5" t="n">
-        <v>20.66</v>
+        <v>25.27</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B93" s="5" t="n">
         <f aca="false">E93*2.3</f>
-        <v>16.238</v>
+        <v>47.518</v>
       </c>
       <c r="C93" s="3" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="E93" s="10" t="n">
-        <v>7.06</v>
+        <v>6.5</v>
+      </c>
+      <c r="E93" s="5" t="n">
+        <v>20.66</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="11" t="s">
+      <c r="A94" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B94" s="5" t="n">
         <f aca="false">E94*2.3</f>
-        <v>22.287</v>
+        <v>16.238</v>
       </c>
       <c r="C94" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E94" s="10" t="n">
-        <v>9.69</v>
+        <v>7.06</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2636,13 +2634,13 @@
       </c>
       <c r="B95" s="5" t="n">
         <f aca="false">E95*2.3</f>
-        <v>27.577</v>
+        <v>22.287</v>
       </c>
       <c r="C95" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E95" s="10" t="n">
-        <v>11.99</v>
+        <v>9.69</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2651,13 +2649,13 @@
       </c>
       <c r="B96" s="5" t="n">
         <f aca="false">E96*2.3</f>
-        <v>37.674</v>
+        <v>27.577</v>
       </c>
       <c r="C96" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E96" s="10" t="n">
-        <v>16.38</v>
+        <v>11.99</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2666,13 +2664,13 @@
       </c>
       <c r="B97" s="5" t="n">
         <f aca="false">E97*2.3</f>
-        <v>42.964</v>
+        <v>37.674</v>
       </c>
       <c r="C97" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E97" s="10" t="n">
-        <v>18.68</v>
+        <v>16.38</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2681,13 +2679,13 @@
       </c>
       <c r="B98" s="5" t="n">
         <f aca="false">E98*2.3</f>
-        <v>32.637</v>
+        <v>42.964</v>
       </c>
       <c r="C98" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E98" s="10" t="n">
-        <v>14.19</v>
+        <v>18.68</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2696,13 +2694,13 @@
       </c>
       <c r="B99" s="5" t="n">
         <f aca="false">E99*2.3</f>
-        <v>37.927</v>
+        <v>32.637</v>
       </c>
       <c r="C99" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E99" s="10" t="n">
-        <v>16.49</v>
+        <v>14.19</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2711,13 +2709,13 @@
       </c>
       <c r="B100" s="5" t="n">
         <f aca="false">E100*2.3</f>
-        <v>44.022</v>
+        <v>37.927</v>
       </c>
       <c r="C100" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E100" s="10" t="n">
-        <v>19.14</v>
+        <v>16.49</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2726,13 +2724,13 @@
       </c>
       <c r="B101" s="5" t="n">
         <f aca="false">E101*2.3</f>
-        <v>49.312</v>
+        <v>44.022</v>
       </c>
       <c r="C101" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E101" s="10" t="n">
-        <v>21.44</v>
+        <v>19.14</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2741,13 +2739,13 @@
       </c>
       <c r="B102" s="5" t="n">
         <f aca="false">E102*2.3</f>
-        <v>24.081</v>
+        <v>49.312</v>
       </c>
       <c r="C102" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E102" s="10" t="n">
-        <v>10.47</v>
+        <v>21.44</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2756,13 +2754,13 @@
       </c>
       <c r="B103" s="5" t="n">
         <f aca="false">E103*2.3</f>
-        <v>47.61</v>
+        <v>24.081</v>
       </c>
       <c r="C103" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E103" s="10" t="n">
-        <v>20.7</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2771,13 +2769,13 @@
       </c>
       <c r="B104" s="5" t="n">
         <f aca="false">E104*2.3</f>
-        <v>24.265</v>
+        <v>47.61</v>
       </c>
       <c r="C104" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E104" s="10" t="n">
-        <v>10.55</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2786,13 +2784,13 @@
       </c>
       <c r="B105" s="5" t="n">
         <f aca="false">E105*2.3</f>
-        <v>21.39</v>
+        <v>24.265</v>
       </c>
       <c r="C105" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E105" s="10" t="n">
-        <v>9.3</v>
+        <v>10.55</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2801,13 +2799,13 @@
       </c>
       <c r="B106" s="5" t="n">
         <f aca="false">E106*2.3</f>
-        <v>24.242</v>
+        <v>21.39</v>
       </c>
       <c r="C106" s="3" t="n">
         <v>3.3</v>
       </c>
-      <c r="E106" s="5" t="n">
-        <v>10.54</v>
+      <c r="E106" s="10" t="n">
+        <v>9.3</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2816,13 +2814,13 @@
       </c>
       <c r="B107" s="5" t="n">
         <f aca="false">E107*2.3</f>
-        <v>37.973</v>
+        <v>24.242</v>
       </c>
       <c r="C107" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E107" s="5" t="n">
-        <v>16.51</v>
+        <v>10.54</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2831,13 +2829,13 @@
       </c>
       <c r="B108" s="5" t="n">
         <f aca="false">E108*2.3</f>
-        <v>22.356</v>
+        <v>37.973</v>
       </c>
       <c r="C108" s="3" t="n">
         <v>3.3</v>
       </c>
-      <c r="E108" s="10" t="n">
-        <v>9.72</v>
+      <c r="E108" s="5" t="n">
+        <v>16.51</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2846,13 +2844,13 @@
       </c>
       <c r="B109" s="5" t="n">
         <f aca="false">E109*2.3</f>
-        <v>29.854</v>
+        <v>22.356</v>
       </c>
       <c r="C109" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E109" s="10" t="n">
-        <v>12.98</v>
+        <v>9.72</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2861,13 +2859,13 @@
       </c>
       <c r="B110" s="5" t="n">
         <f aca="false">E110*2.3</f>
-        <v>38.502</v>
+        <v>29.854</v>
       </c>
       <c r="C110" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E110" s="10" t="n">
-        <v>16.74</v>
+        <v>12.98</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2876,13 +2874,13 @@
       </c>
       <c r="B111" s="5" t="n">
         <f aca="false">E111*2.3</f>
-        <v>43.424</v>
+        <v>38.502</v>
       </c>
       <c r="C111" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E111" s="10" t="n">
-        <v>18.88</v>
+        <v>16.74</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2891,13 +2889,13 @@
       </c>
       <c r="B112" s="5" t="n">
         <f aca="false">E112*2.3</f>
-        <v>52.095</v>
+        <v>43.424</v>
       </c>
       <c r="C112" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E112" s="10" t="n">
-        <v>22.65</v>
+        <v>18.88</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2906,13 +2904,13 @@
       </c>
       <c r="B113" s="5" t="n">
         <f aca="false">E113*2.3</f>
-        <v>37.536</v>
+        <v>52.095</v>
       </c>
       <c r="C113" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E113" s="10" t="n">
-        <v>16.32</v>
+        <v>22.65</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2921,13 +2919,13 @@
       </c>
       <c r="B114" s="5" t="n">
         <f aca="false">E114*2.3</f>
-        <v>46.23</v>
+        <v>37.536</v>
       </c>
       <c r="C114" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E114" s="10" t="n">
-        <v>20.1</v>
+        <v>16.32</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2936,13 +2934,13 @@
       </c>
       <c r="B115" s="5" t="n">
         <f aca="false">E115*2.3</f>
-        <v>48.691</v>
+        <v>46.23</v>
       </c>
       <c r="C115" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E115" s="10" t="n">
-        <v>21.17</v>
+        <v>20.1</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2951,13 +2949,13 @@
       </c>
       <c r="B116" s="5" t="n">
         <f aca="false">E116*2.3</f>
-        <v>57.362</v>
+        <v>48.691</v>
       </c>
       <c r="C116" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E116" s="10" t="n">
-        <v>24.94</v>
+        <v>21.17</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2966,13 +2964,13 @@
       </c>
       <c r="B117" s="5" t="n">
         <f aca="false">E117*2.3</f>
-        <v>29.946</v>
+        <v>57.362</v>
       </c>
       <c r="C117" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E117" s="10" t="n">
-        <v>13.02</v>
+        <v>24.94</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2981,13 +2979,13 @@
       </c>
       <c r="B118" s="5" t="n">
         <f aca="false">E118*2.3</f>
-        <v>55.499</v>
+        <v>29.946</v>
       </c>
       <c r="C118" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E118" s="10" t="n">
-        <v>24.13</v>
+        <v>13.02</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2996,13 +2994,13 @@
       </c>
       <c r="B119" s="5" t="n">
         <f aca="false">E119*2.3</f>
-        <v>32.223</v>
+        <v>55.499</v>
       </c>
       <c r="C119" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E119" s="10" t="n">
-        <v>14.01</v>
+        <v>24.13</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3011,13 +3009,13 @@
       </c>
       <c r="B120" s="5" t="n">
         <f aca="false">E120*2.3</f>
-        <v>28.198</v>
+        <v>32.223</v>
       </c>
       <c r="C120" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E120" s="10" t="n">
-        <v>12.26</v>
+        <v>14.01</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3026,13 +3024,13 @@
       </c>
       <c r="B121" s="5" t="n">
         <f aca="false">E121*2.3</f>
-        <v>29.532</v>
+        <v>28.198</v>
       </c>
       <c r="C121" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="E121" s="10" t="n">
-        <v>12.84</v>
+        <v>12.26</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3041,13 +3039,13 @@
       </c>
       <c r="B122" s="5" t="n">
         <f aca="false">E122*2.3</f>
-        <v>41.101</v>
+        <v>29.532</v>
       </c>
       <c r="C122" s="3" t="n">
         <v>3.3</v>
       </c>
-      <c r="E122" s="12" t="n">
-        <v>17.87</v>
+      <c r="E122" s="10" t="n">
+        <v>12.84</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3056,13 +3054,13 @@
       </c>
       <c r="B123" s="5" t="n">
         <f aca="false">E123*2.3</f>
-        <v>23.529</v>
+        <v>41.101</v>
       </c>
       <c r="C123" s="3" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="E123" s="10" t="n">
-        <v>10.23</v>
+        <v>3.3</v>
+      </c>
+      <c r="E123" s="12" t="n">
+        <v>17.87</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3071,13 +3069,13 @@
       </c>
       <c r="B124" s="5" t="n">
         <f aca="false">E124*2.3</f>
-        <v>46.552</v>
+        <v>23.529</v>
       </c>
       <c r="C124" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E124" s="10" t="n">
-        <v>20.24</v>
+        <v>10.23</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3086,13 +3084,13 @@
       </c>
       <c r="B125" s="5" t="n">
         <f aca="false">E125*2.3</f>
-        <v>47.472</v>
+        <v>46.552</v>
       </c>
       <c r="C125" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E125" s="10" t="n">
-        <v>20.64</v>
+        <v>20.24</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3101,13 +3099,13 @@
       </c>
       <c r="B126" s="5" t="n">
         <f aca="false">E126*2.3</f>
-        <v>35.397</v>
+        <v>47.472</v>
       </c>
       <c r="C126" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E126" s="10" t="n">
-        <v>15.39</v>
+        <v>20.64</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3116,13 +3114,13 @@
       </c>
       <c r="B127" s="5" t="n">
         <f aca="false">E127*2.3</f>
-        <v>34.017</v>
+        <v>35.397</v>
       </c>
       <c r="C127" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E127" s="10" t="n">
-        <v>14.79</v>
+        <v>15.39</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3131,13 +3129,13 @@
       </c>
       <c r="B128" s="5" t="n">
         <f aca="false">E128*2.3</f>
-        <v>64.676</v>
+        <v>34.017</v>
       </c>
       <c r="C128" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E128" s="10" t="n">
-        <v>28.12</v>
+        <v>14.79</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3146,13 +3144,13 @@
       </c>
       <c r="B129" s="5" t="n">
         <f aca="false">E129*2.3</f>
-        <v>27.922</v>
+        <v>64.676</v>
       </c>
       <c r="C129" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E129" s="10" t="n">
-        <v>12.14</v>
+        <v>28.12</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3161,13 +3159,13 @@
       </c>
       <c r="B130" s="5" t="n">
         <f aca="false">E130*2.3</f>
-        <v>34.891</v>
+        <v>27.922</v>
       </c>
       <c r="C130" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E130" s="10" t="n">
-        <v>15.17</v>
+        <v>12.14</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3176,13 +3174,13 @@
       </c>
       <c r="B131" s="5" t="n">
         <f aca="false">E131*2.3</f>
-        <v>53.13</v>
+        <v>34.891</v>
       </c>
       <c r="C131" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E131" s="10" t="n">
-        <v>23.1</v>
+        <v>15.17</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3191,13 +3189,13 @@
       </c>
       <c r="B132" s="5" t="n">
         <f aca="false">E132*2.3</f>
-        <v>53.981</v>
+        <v>53.13</v>
       </c>
       <c r="C132" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E132" s="10" t="n">
-        <v>23.47</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3206,13 +3204,13 @@
       </c>
       <c r="B133" s="5" t="n">
         <f aca="false">E133*2.3</f>
-        <v>42.481</v>
+        <v>53.981</v>
       </c>
       <c r="C133" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E133" s="10" t="n">
-        <v>18.47</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3221,13 +3219,13 @@
       </c>
       <c r="B134" s="5" t="n">
         <f aca="false">E134*2.3</f>
-        <v>39.606</v>
+        <v>42.481</v>
       </c>
       <c r="C134" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E134" s="10" t="n">
-        <v>17.22</v>
+        <v>18.47</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3236,13 +3234,13 @@
       </c>
       <c r="B135" s="5" t="n">
         <f aca="false">E135*2.3</f>
-        <v>74.98</v>
+        <v>39.606</v>
       </c>
       <c r="C135" s="3" t="n">
         <v>4.1</v>
       </c>
       <c r="E135" s="10" t="n">
-        <v>32.6</v>
+        <v>17.22</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3251,13 +3249,13 @@
       </c>
       <c r="B136" s="5" t="n">
         <f aca="false">E136*2.3</f>
-        <v>25.921</v>
+        <v>74.98</v>
       </c>
       <c r="C136" s="3" t="n">
-        <v>4.9</v>
+        <v>4.1</v>
       </c>
       <c r="E136" s="10" t="n">
-        <v>11.27</v>
+        <v>32.6</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3266,13 +3264,13 @@
       </c>
       <c r="B137" s="5" t="n">
         <f aca="false">E137*2.3</f>
-        <v>33.948</v>
+        <v>25.921</v>
       </c>
       <c r="C137" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E137" s="10" t="n">
-        <v>14.76</v>
+        <v>11.27</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3281,13 +3279,13 @@
       </c>
       <c r="B138" s="5" t="n">
         <f aca="false">E138*2.3</f>
-        <v>46.414</v>
+        <v>33.948</v>
       </c>
       <c r="C138" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E138" s="10" t="n">
-        <v>20.18</v>
+        <v>14.76</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3296,13 +3294,13 @@
       </c>
       <c r="B139" s="5" t="n">
         <f aca="false">E139*2.3</f>
-        <v>29.992</v>
+        <v>46.414</v>
       </c>
       <c r="C139" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E139" s="10" t="n">
-        <v>13.04</v>
+        <v>20.18</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3311,13 +3309,13 @@
       </c>
       <c r="B140" s="5" t="n">
         <f aca="false">E140*2.3</f>
-        <v>36.961</v>
+        <v>29.992</v>
       </c>
       <c r="C140" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E140" s="10" t="n">
-        <v>16.07</v>
+        <v>13.04</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3326,13 +3324,13 @@
       </c>
       <c r="B141" s="5" t="n">
         <f aca="false">E141*2.3</f>
-        <v>39.951</v>
+        <v>36.961</v>
       </c>
       <c r="C141" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E141" s="10" t="n">
-        <v>17.37</v>
+        <v>16.07</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3341,13 +3339,13 @@
       </c>
       <c r="B142" s="5" t="n">
         <f aca="false">E142*2.3</f>
-        <v>46.92</v>
+        <v>39.951</v>
       </c>
       <c r="C142" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E142" s="10" t="n">
-        <v>20.4</v>
+        <v>17.37</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3356,13 +3354,13 @@
       </c>
       <c r="B143" s="5" t="n">
         <f aca="false">E143*2.3</f>
-        <v>46.897</v>
+        <v>46.92</v>
       </c>
       <c r="C143" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E143" s="10" t="n">
-        <v>20.39</v>
+        <v>20.4</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3371,13 +3369,13 @@
       </c>
       <c r="B144" s="5" t="n">
         <f aca="false">E144*2.3</f>
-        <v>53.866</v>
+        <v>46.897</v>
       </c>
       <c r="C144" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E144" s="10" t="n">
-        <v>23.42</v>
+        <v>20.39</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3386,13 +3384,13 @@
       </c>
       <c r="B145" s="5" t="n">
         <f aca="false">E145*2.3</f>
-        <v>32.154</v>
+        <v>53.866</v>
       </c>
       <c r="C145" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E145" s="10" t="n">
-        <v>13.98</v>
+        <v>23.42</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3401,13 +3399,13 @@
       </c>
       <c r="B146" s="5" t="n">
         <f aca="false">E146*2.3</f>
-        <v>28.796</v>
+        <v>32.154</v>
       </c>
       <c r="C146" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E146" s="10" t="n">
-        <v>12.52</v>
+        <v>13.98</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3416,13 +3414,13 @@
       </c>
       <c r="B147" s="5" t="n">
         <f aca="false">E147*2.3</f>
-        <v>28.037</v>
+        <v>28.796</v>
       </c>
       <c r="C147" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E147" s="10" t="n">
-        <v>12.19</v>
+        <v>12.52</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3431,13 +3429,13 @@
       </c>
       <c r="B148" s="5" t="n">
         <f aca="false">E148*2.3</f>
-        <v>42.826</v>
+        <v>28.037</v>
       </c>
       <c r="C148" s="3" t="n">
         <v>4.9</v>
       </c>
-      <c r="E148" s="12" t="n">
-        <v>18.62</v>
+      <c r="E148" s="10" t="n">
+        <v>12.19</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3446,13 +3444,13 @@
       </c>
       <c r="B149" s="5" t="n">
         <f aca="false">E149*2.3</f>
-        <v>29.601</v>
+        <v>42.826</v>
       </c>
       <c r="C149" s="3" t="n">
         <v>4.9</v>
       </c>
-      <c r="E149" s="10" t="n">
-        <v>12.87</v>
+      <c r="E149" s="12" t="n">
+        <v>18.62</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3461,13 +3459,13 @@
       </c>
       <c r="B150" s="5" t="n">
         <f aca="false">E150*2.3</f>
-        <v>40.273</v>
+        <v>29.601</v>
       </c>
       <c r="C150" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E150" s="10" t="n">
-        <v>17.51</v>
+        <v>12.87</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3476,13 +3474,13 @@
       </c>
       <c r="B151" s="5" t="n">
         <f aca="false">E151*2.3</f>
-        <v>52.072</v>
+        <v>40.273</v>
       </c>
       <c r="C151" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E151" s="10" t="n">
-        <v>22.64</v>
+        <v>17.51</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3491,13 +3489,13 @@
       </c>
       <c r="B152" s="5" t="n">
         <f aca="false">E152*2.3</f>
-        <v>34.822</v>
+        <v>52.072</v>
       </c>
       <c r="C152" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E152" s="10" t="n">
-        <v>15.14</v>
+        <v>22.64</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3506,13 +3504,13 @@
       </c>
       <c r="B153" s="5" t="n">
         <f aca="false">E153*2.3</f>
-        <v>39.813</v>
+        <v>34.822</v>
       </c>
       <c r="C153" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E153" s="10" t="n">
-        <v>17.31</v>
+        <v>15.14</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3521,13 +3519,13 @@
       </c>
       <c r="B154" s="5" t="n">
         <f aca="false">E154*2.3</f>
-        <v>43.217</v>
+        <v>39.813</v>
       </c>
       <c r="C154" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E154" s="10" t="n">
-        <v>18.79</v>
+        <v>17.31</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3536,13 +3534,13 @@
       </c>
       <c r="B155" s="5" t="n">
         <f aca="false">E155*2.3</f>
-        <v>48.208</v>
+        <v>43.217</v>
       </c>
       <c r="C155" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E155" s="10" t="n">
-        <v>20.96</v>
+        <v>18.79</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3551,13 +3549,13 @@
       </c>
       <c r="B156" s="5" t="n">
         <f aca="false">E156*2.3</f>
-        <v>49.933</v>
+        <v>48.208</v>
       </c>
       <c r="C156" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E156" s="10" t="n">
-        <v>21.71</v>
+        <v>20.96</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3566,13 +3564,13 @@
       </c>
       <c r="B157" s="5" t="n">
         <f aca="false">E157*2.3</f>
-        <v>54.924</v>
+        <v>49.933</v>
       </c>
       <c r="C157" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E157" s="10" t="n">
-        <v>23.88</v>
+        <v>21.71</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3581,13 +3579,13 @@
       </c>
       <c r="B158" s="5" t="n">
         <f aca="false">E158*2.3</f>
-        <v>37.973</v>
+        <v>54.924</v>
       </c>
       <c r="C158" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E158" s="10" t="n">
-        <v>16.51</v>
+        <v>23.88</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3596,13 +3594,13 @@
       </c>
       <c r="B159" s="5" t="n">
         <f aca="false">E159*2.3</f>
-        <v>37.007</v>
+        <v>37.973</v>
       </c>
       <c r="C159" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E159" s="10" t="n">
-        <v>16.09</v>
+        <v>16.51</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3611,13 +3609,13 @@
       </c>
       <c r="B160" s="5" t="n">
         <f aca="false">E160*2.3</f>
-        <v>35.558</v>
+        <v>37.007</v>
       </c>
       <c r="C160" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="E160" s="10" t="n">
-        <v>15.46</v>
+        <v>16.09</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3626,28 +3624,28 @@
       </c>
       <c r="B161" s="5" t="n">
         <f aca="false">E161*2.3</f>
-        <v>44.712</v>
+        <v>35.558</v>
       </c>
       <c r="C161" s="3" t="n">
         <v>4.9</v>
       </c>
-      <c r="E161" s="12" t="n">
-        <v>19.44</v>
+      <c r="E161" s="10" t="n">
+        <v>15.46</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="13" t="s">
+      <c r="A162" s="11" t="s">
         <v>164</v>
       </c>
       <c r="B162" s="5" t="n">
         <f aca="false">E162*2.3</f>
-        <v>26.22</v>
+        <v>44.712</v>
       </c>
       <c r="C162" s="3" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="E162" s="10" t="n">
-        <v>11.4</v>
+        <v>4.9</v>
+      </c>
+      <c r="E162" s="12" t="n">
+        <v>19.44</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3656,13 +3654,13 @@
       </c>
       <c r="B163" s="5" t="n">
         <f aca="false">E163*2.3</f>
-        <v>35.604</v>
+        <v>26.22</v>
       </c>
       <c r="C163" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E163" s="10" t="n">
-        <v>15.48</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3671,13 +3669,13 @@
       </c>
       <c r="B164" s="5" t="n">
         <f aca="false">E164*2.3</f>
-        <v>41.193</v>
+        <v>35.604</v>
       </c>
       <c r="C164" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E164" s="10" t="n">
-        <v>17.91</v>
+        <v>15.48</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3686,13 +3684,13 @@
       </c>
       <c r="B165" s="5" t="n">
         <f aca="false">E165*2.3</f>
-        <v>48.53</v>
+        <v>41.193</v>
       </c>
       <c r="C165" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E165" s="10" t="n">
-        <v>21.1</v>
+        <v>17.91</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3701,13 +3699,13 @@
       </c>
       <c r="B166" s="5" t="n">
         <f aca="false">E166*2.3</f>
-        <v>61.755</v>
+        <v>48.53</v>
       </c>
       <c r="C166" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E166" s="10" t="n">
-        <v>26.85</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3731,13 +3729,13 @@
       </c>
       <c r="B168" s="5" t="n">
         <f aca="false">E168*2.3</f>
-        <v>69.092</v>
+        <v>61.755</v>
       </c>
       <c r="C168" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E168" s="10" t="n">
-        <v>30.04</v>
+        <v>26.85</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3746,13 +3744,13 @@
       </c>
       <c r="B169" s="5" t="n">
         <f aca="false">E169*2.3</f>
-        <v>42.941</v>
+        <v>69.092</v>
       </c>
       <c r="C169" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E169" s="10" t="n">
-        <v>18.67</v>
+        <v>30.04</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3761,13 +3759,13 @@
       </c>
       <c r="B170" s="5" t="n">
         <f aca="false">E170*2.3</f>
-        <v>50.715</v>
+        <v>42.941</v>
       </c>
       <c r="C170" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E170" s="10" t="n">
-        <v>22.05</v>
+        <v>18.67</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3776,13 +3774,13 @@
       </c>
       <c r="B171" s="5" t="n">
         <f aca="false">E171*2.3</f>
-        <v>37.329</v>
+        <v>50.715</v>
       </c>
       <c r="C171" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E171" s="10" t="n">
-        <v>16.23</v>
+        <v>22.05</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3791,13 +3789,13 @@
       </c>
       <c r="B172" s="5" t="n">
         <f aca="false">E172*2.3</f>
-        <v>42.044</v>
+        <v>37.329</v>
       </c>
       <c r="C172" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E172" s="10" t="n">
-        <v>18.28</v>
+        <v>16.23</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3806,13 +3804,13 @@
       </c>
       <c r="B173" s="5" t="n">
         <f aca="false">E173*2.3</f>
-        <v>45.954</v>
+        <v>42.044</v>
       </c>
       <c r="C173" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E173" s="10" t="n">
-        <v>19.98</v>
+        <v>18.28</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3821,13 +3819,13 @@
       </c>
       <c r="B174" s="5" t="n">
         <f aca="false">E174*2.3</f>
-        <v>49.956</v>
+        <v>45.954</v>
       </c>
       <c r="C174" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E174" s="10" t="n">
-        <v>21.72</v>
+        <v>19.98</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3836,13 +3834,13 @@
       </c>
       <c r="B175" s="5" t="n">
         <f aca="false">E175*2.3</f>
-        <v>54.694</v>
+        <v>49.956</v>
       </c>
       <c r="C175" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E175" s="10" t="n">
-        <v>23.78</v>
+        <v>21.72</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3851,13 +3849,13 @@
       </c>
       <c r="B176" s="5" t="n">
         <f aca="false">E176*2.3</f>
-        <v>41.515</v>
+        <v>54.694</v>
       </c>
       <c r="C176" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E176" s="10" t="n">
-        <v>18.05</v>
+        <v>23.78</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3866,13 +3864,13 @@
       </c>
       <c r="B177" s="5" t="n">
         <f aca="false">E177*2.3</f>
-        <v>47.127</v>
+        <v>41.515</v>
       </c>
       <c r="C177" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E177" s="10" t="n">
-        <v>20.49</v>
+        <v>18.05</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3881,13 +3879,13 @@
       </c>
       <c r="B178" s="5" t="n">
         <f aca="false">E178*2.3</f>
-        <v>52.21</v>
+        <v>47.127</v>
       </c>
       <c r="C178" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E178" s="10" t="n">
-        <v>22.7</v>
+        <v>20.49</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3896,13 +3894,13 @@
       </c>
       <c r="B179" s="5" t="n">
         <f aca="false">E179*2.3</f>
-        <v>59.984</v>
+        <v>52.21</v>
       </c>
       <c r="C179" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E179" s="10" t="n">
-        <v>26.08</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3911,13 +3909,13 @@
       </c>
       <c r="B180" s="5" t="n">
         <f aca="false">E180*2.3</f>
-        <v>46.598</v>
+        <v>59.984</v>
       </c>
       <c r="C180" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E180" s="10" t="n">
-        <v>20.26</v>
+        <v>26.08</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3926,13 +3924,13 @@
       </c>
       <c r="B181" s="5" t="n">
         <f aca="false">E181*2.3</f>
-        <v>51.336</v>
+        <v>46.598</v>
       </c>
       <c r="C181" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E181" s="10" t="n">
-        <v>22.32</v>
+        <v>20.26</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3941,13 +3939,13 @@
       </c>
       <c r="B182" s="5" t="n">
         <f aca="false">E182*2.3</f>
-        <v>52.348</v>
+        <v>51.336</v>
       </c>
       <c r="C182" s="3" t="n">
-        <v>8.3</v>
+        <v>6.5</v>
       </c>
       <c r="E182" s="10" t="n">
-        <v>22.76</v>
+        <v>22.32</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3956,13 +3954,13 @@
       </c>
       <c r="B183" s="5" t="n">
         <f aca="false">E183*2.3</f>
-        <v>57.937</v>
+        <v>52.348</v>
       </c>
       <c r="C183" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E183" s="10" t="n">
-        <v>25.19</v>
+        <v>22.76</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3971,13 +3969,13 @@
       </c>
       <c r="B184" s="5" t="n">
         <f aca="false">E184*2.3</f>
-        <v>65.274</v>
+        <v>57.937</v>
       </c>
       <c r="C184" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E184" s="10" t="n">
-        <v>28.38</v>
+        <v>25.19</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3986,13 +3984,13 @@
       </c>
       <c r="B185" s="5" t="n">
         <f aca="false">E185*2.3</f>
-        <v>59.662</v>
+        <v>65.274</v>
       </c>
       <c r="C185" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E185" s="10" t="n">
-        <v>25.94</v>
+        <v>28.38</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4001,13 +3999,13 @@
       </c>
       <c r="B186" s="5" t="n">
         <f aca="false">E186*2.3</f>
-        <v>58.788</v>
+        <v>59.662</v>
       </c>
       <c r="C186" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E186" s="10" t="n">
-        <v>25.56</v>
+        <v>25.94</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4016,13 +4014,13 @@
       </c>
       <c r="B187" s="5" t="n">
         <f aca="false">E187*2.3</f>
-        <v>54.073</v>
+        <v>58.788</v>
       </c>
       <c r="C187" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E187" s="10" t="n">
-        <v>23.51</v>
+        <v>25.56</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4031,13 +4029,13 @@
       </c>
       <c r="B188" s="5" t="n">
         <f aca="false">E188*2.3</f>
-        <v>58.788</v>
+        <v>54.073</v>
       </c>
       <c r="C188" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E188" s="10" t="n">
-        <v>25.56</v>
+        <v>23.51</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4046,13 +4044,13 @@
       </c>
       <c r="B189" s="5" t="n">
         <f aca="false">E189*2.3</f>
-        <v>32.154</v>
+        <v>58.788</v>
       </c>
       <c r="C189" s="3" t="n">
-        <v>6.5</v>
+        <v>8.3</v>
       </c>
       <c r="E189" s="10" t="n">
-        <v>13.98</v>
+        <v>25.56</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4061,13 +4059,13 @@
       </c>
       <c r="B190" s="5" t="n">
         <f aca="false">E190*2.3</f>
-        <v>54.717</v>
+        <v>32.154</v>
       </c>
       <c r="C190" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E190" s="10" t="n">
-        <v>23.79</v>
+        <v>13.98</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4091,13 +4089,13 @@
       </c>
       <c r="B192" s="5" t="n">
         <f aca="false">E192*2.3</f>
-        <v>69.207</v>
+        <v>54.717</v>
       </c>
       <c r="C192" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E192" s="10" t="n">
-        <v>30.09</v>
+        <v>23.79</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4106,43 +4104,43 @@
       </c>
       <c r="B193" s="5" t="n">
         <f aca="false">E193*2.3</f>
-        <v>40.756</v>
+        <v>69.207</v>
       </c>
       <c r="C193" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E193" s="10" t="n">
-        <v>17.72</v>
+        <v>30.09</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="14" t="s">
+      <c r="A194" s="13" t="s">
         <v>196</v>
       </c>
       <c r="B194" s="5" t="n">
         <f aca="false">E194*2.3</f>
-        <v>42.964</v>
+        <v>40.756</v>
       </c>
       <c r="C194" s="3" t="n">
         <v>6.5</v>
       </c>
-      <c r="E194" s="12" t="n">
-        <v>18.68</v>
+      <c r="E194" s="10" t="n">
+        <v>17.72</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A195" s="13" t="s">
+      <c r="A195" s="14" t="s">
         <v>197</v>
       </c>
       <c r="B195" s="5" t="n">
         <f aca="false">E195*2.3</f>
-        <v>30.59</v>
+        <v>42.964</v>
       </c>
       <c r="C195" s="3" t="n">
         <v>6.5</v>
       </c>
-      <c r="E195" s="15" t="n">
-        <v>13.3</v>
+      <c r="E195" s="12" t="n">
+        <v>18.68</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4151,13 +4149,13 @@
       </c>
       <c r="B196" s="5" t="n">
         <f aca="false">E196*2.3</f>
-        <v>39.951</v>
+        <v>30.59</v>
       </c>
       <c r="C196" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E196" s="15" t="n">
-        <v>17.37</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4166,13 +4164,13 @@
       </c>
       <c r="B197" s="5" t="n">
         <f aca="false">E197*2.3</f>
-        <v>45.701</v>
+        <v>39.951</v>
       </c>
       <c r="C197" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E197" s="15" t="n">
-        <v>19.87</v>
+        <v>17.37</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4181,13 +4179,13 @@
       </c>
       <c r="B198" s="5" t="n">
         <f aca="false">E198*2.3</f>
-        <v>53.222</v>
+        <v>45.701</v>
       </c>
       <c r="C198" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E198" s="15" t="n">
-        <v>23.14</v>
+        <v>19.87</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4196,13 +4194,13 @@
       </c>
       <c r="B199" s="5" t="n">
         <f aca="false">E199*2.3</f>
-        <v>64.354</v>
+        <v>53.222</v>
       </c>
       <c r="C199" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E199" s="15" t="n">
-        <v>27.98</v>
+        <v>23.14</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4226,13 +4224,13 @@
       </c>
       <c r="B201" s="5" t="n">
         <f aca="false">E201*2.3</f>
-        <v>71.875</v>
+        <v>64.354</v>
       </c>
       <c r="C201" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E201" s="15" t="n">
-        <v>31.25</v>
+        <v>27.98</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4241,13 +4239,13 @@
       </c>
       <c r="B202" s="5" t="n">
         <f aca="false">E202*2.3</f>
-        <v>49.197</v>
+        <v>71.875</v>
       </c>
       <c r="C202" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E202" s="15" t="n">
-        <v>21.39</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4256,13 +4254,13 @@
       </c>
       <c r="B203" s="5" t="n">
         <f aca="false">E203*2.3</f>
-        <v>57.983</v>
+        <v>49.197</v>
       </c>
       <c r="C203" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E203" s="15" t="n">
-        <v>25.21</v>
+        <v>21.39</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4271,13 +4269,13 @@
       </c>
       <c r="B204" s="5" t="n">
         <f aca="false">E204*2.3</f>
-        <v>42.941</v>
+        <v>57.983</v>
       </c>
       <c r="C204" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E204" s="15" t="n">
-        <v>18.67</v>
+        <v>25.21</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4286,13 +4284,13 @@
       </c>
       <c r="B205" s="5" t="n">
         <f aca="false">E205*2.3</f>
-        <v>49.036</v>
+        <v>42.941</v>
       </c>
       <c r="C205" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E205" s="15" t="n">
-        <v>21.32</v>
+        <v>18.67</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4301,13 +4299,13 @@
       </c>
       <c r="B206" s="5" t="n">
         <f aca="false">E206*2.3</f>
-        <v>54.326</v>
+        <v>49.036</v>
       </c>
       <c r="C206" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E206" s="15" t="n">
-        <v>23.62</v>
+        <v>21.32</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4316,13 +4314,13 @@
       </c>
       <c r="B207" s="5" t="n">
         <f aca="false">E207*2.3</f>
-        <v>56.373</v>
+        <v>54.326</v>
       </c>
       <c r="C207" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E207" s="15" t="n">
-        <v>24.51</v>
+        <v>23.62</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4331,13 +4329,13 @@
       </c>
       <c r="B208" s="5" t="n">
         <f aca="false">E208*2.3</f>
-        <v>62.491</v>
+        <v>56.373</v>
       </c>
       <c r="C208" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E208" s="15" t="n">
-        <v>27.17</v>
+        <v>24.51</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4346,13 +4344,13 @@
       </c>
       <c r="B209" s="5" t="n">
         <f aca="false">E209*2.3</f>
-        <v>47.334</v>
+        <v>62.491</v>
       </c>
       <c r="C209" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E209" s="15" t="n">
-        <v>20.58</v>
+        <v>27.17</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4361,13 +4359,13 @@
       </c>
       <c r="B210" s="5" t="n">
         <f aca="false">E210*2.3</f>
-        <v>53.084</v>
+        <v>47.334</v>
       </c>
       <c r="C210" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E210" s="15" t="n">
-        <v>23.08</v>
+        <v>20.58</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4376,13 +4374,13 @@
       </c>
       <c r="B211" s="5" t="n">
         <f aca="false">E211*2.3</f>
-        <v>56.58</v>
+        <v>53.084</v>
       </c>
       <c r="C211" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E211" s="15" t="n">
-        <v>24.6</v>
+        <v>23.08</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4391,13 +4389,13 @@
       </c>
       <c r="B212" s="5" t="n">
         <f aca="false">E212*2.3</f>
-        <v>65.366</v>
+        <v>56.58</v>
       </c>
       <c r="C212" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E212" s="15" t="n">
-        <v>28.42</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4406,13 +4404,13 @@
       </c>
       <c r="B213" s="5" t="n">
         <f aca="false">E213*2.3</f>
-        <v>50.439</v>
+        <v>65.366</v>
       </c>
       <c r="C213" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E213" s="15" t="n">
-        <v>21.93</v>
+        <v>28.42</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4421,13 +4419,13 @@
       </c>
       <c r="B214" s="5" t="n">
         <f aca="false">E214*2.3</f>
-        <v>56.534</v>
+        <v>50.439</v>
       </c>
       <c r="C214" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E214" s="15" t="n">
-        <v>24.58</v>
+        <v>21.93</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4436,13 +4434,13 @@
       </c>
       <c r="B215" s="5" t="n">
         <f aca="false">E215*2.3</f>
-        <v>54.786</v>
+        <v>56.534</v>
       </c>
       <c r="C215" s="3" t="n">
-        <v>8.3</v>
+        <v>6.5</v>
       </c>
       <c r="E215" s="15" t="n">
-        <v>23.82</v>
+        <v>24.58</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4451,13 +4449,13 @@
       </c>
       <c r="B216" s="5" t="n">
         <f aca="false">E216*2.3</f>
-        <v>60.329</v>
+        <v>54.786</v>
       </c>
       <c r="C216" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E216" s="15" t="n">
-        <v>26.23</v>
+        <v>23.82</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4466,13 +4464,13 @@
       </c>
       <c r="B217" s="5" t="n">
         <f aca="false">E217*2.3</f>
-        <v>67.85</v>
+        <v>60.329</v>
       </c>
       <c r="C217" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E217" s="15" t="n">
-        <v>29.5</v>
+        <v>26.23</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4481,13 +4479,13 @@
       </c>
       <c r="B218" s="5" t="n">
         <f aca="false">E218*2.3</f>
-        <v>63.825</v>
+        <v>67.85</v>
       </c>
       <c r="C218" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E218" s="15" t="n">
-        <v>27.75</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4496,13 +4494,13 @@
       </c>
       <c r="B219" s="5" t="n">
         <f aca="false">E219*2.3</f>
-        <v>63.779</v>
+        <v>63.825</v>
       </c>
       <c r="C219" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E219" s="15" t="n">
-        <v>27.73</v>
+        <v>27.75</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4511,13 +4509,13 @@
       </c>
       <c r="B220" s="5" t="n">
         <f aca="false">E220*2.3</f>
-        <v>57.661</v>
+        <v>63.779</v>
       </c>
       <c r="C220" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E220" s="15" t="n">
-        <v>25.07</v>
+        <v>27.73</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4526,13 +4524,13 @@
       </c>
       <c r="B221" s="5" t="n">
         <f aca="false">E221*2.3</f>
-        <v>63.779</v>
+        <v>57.661</v>
       </c>
       <c r="C221" s="3" t="n">
         <v>8.3</v>
       </c>
       <c r="E221" s="15" t="n">
-        <v>27.73</v>
+        <v>25.07</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4541,13 +4539,13 @@
       </c>
       <c r="B222" s="5" t="n">
         <f aca="false">E222*2.3</f>
-        <v>37.973</v>
+        <v>63.779</v>
       </c>
       <c r="C222" s="3" t="n">
-        <v>6.5</v>
+        <v>8.3</v>
       </c>
       <c r="E222" s="15" t="n">
-        <v>16.51</v>
+        <v>27.73</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4556,13 +4554,13 @@
       </c>
       <c r="B223" s="5" t="n">
         <f aca="false">E223*2.3</f>
-        <v>59.593</v>
+        <v>37.973</v>
       </c>
       <c r="C223" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E223" s="15" t="n">
-        <v>25.91</v>
+        <v>16.51</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4586,13 +4584,13 @@
       </c>
       <c r="B225" s="5" t="n">
         <f aca="false">E225*2.3</f>
-        <v>78.292</v>
+        <v>59.593</v>
       </c>
       <c r="C225" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E225" s="15" t="n">
-        <v>34.04</v>
+        <v>25.91</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4601,31 +4599,45 @@
       </c>
       <c r="B226" s="5" t="n">
         <f aca="false">E226*2.3</f>
-        <v>45.839</v>
+        <v>78.292</v>
       </c>
       <c r="C226" s="3" t="n">
         <v>6.5</v>
       </c>
       <c r="E226" s="15" t="n">
-        <v>19.93</v>
+        <v>34.04</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A227" s="14" t="s">
+      <c r="A227" s="13" t="s">
         <v>229</v>
       </c>
       <c r="B227" s="5" t="n">
         <f aca="false">E227*2.3</f>
+        <v>45.839</v>
+      </c>
+      <c r="C227" s="3" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E227" s="15" t="n">
+        <v>19.93</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A228" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B228" s="5" t="n">
+        <f aca="false">E228*2.3</f>
         <v>45.218</v>
       </c>
-      <c r="C227" s="3" t="n">
+      <c r="C228" s="3" t="n">
         <v>8.3</v>
       </c>
-      <c r="E227" s="16" t="n">
+      <c r="E228" s="16" t="n">
         <v>19.66</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5335,7 +5347,7 @@
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>